<commit_message>
zwischenstand ra + db
</commit_message>
<xml_diff>
--- a/2/Rechnerarchitektur/Aufgabe 4/Übung 4_2 - Pipeline_Vorlage.xlsx
+++ b/2/Rechnerarchitektur/Aufgabe 4/Übung 4_2 - Pipeline_Vorlage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tombo\HTWG\AIN\2\Rechnerarchitektur\Aufgabe 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750FEF15-764F-42C4-ADF5-C04BD973D444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6494980D-86B6-40C9-ADD2-DC2FDFABE94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pipeline" sheetId="3" r:id="rId1"/>

</xml_diff>